<commit_message>
nov 7 button updates
</commit_message>
<xml_diff>
--- a/SRC 2/surveys nov 7/Survey Statements/LTC_Survey_Data_2021_to_Present.xlsx
+++ b/SRC 2/surveys nov 7/Survey Statements/LTC_Survey_Data_2021_to_Present.xlsx
@@ -675,7 +675,7 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>R 147,R147,R 136,R136,R162,R 162</t>
+          <t>R 162,R162,R136,R 147,R147,R 136</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
@@ -799,7 +799,7 @@
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>V. RESIDENT CARE,IX. PHYSICAL</t>
+          <t>IX. PHYSICAL,V. RESIDENT CARE</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
@@ -933,7 +933,7 @@
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>R128,R145,R200,R136,R179</t>
+          <t>R145,R128,R136,R179,R200</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
@@ -948,7 +948,7 @@
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>D, F</t>
+          <t>F, D</t>
         </is>
       </c>
       <c r="AA4" t="inlineStr">
@@ -1455,7 +1455,7 @@
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>R266,R100,R 266</t>
+          <t>R 266,R100,R266</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
@@ -1584,7 +1584,7 @@
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>R126,R190,R179,R213</t>
+          <t>R213,R190,R126,R179</t>
         </is>
       </c>
       <c r="X9" t="inlineStr">
@@ -1709,7 +1709,7 @@
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>R 251,R145,R 145,R999,R 247,R251,R247</t>
+          <t>R999,R 247,R251,R 251,R247,R 145,R145</t>
         </is>
       </c>
       <c r="X10" t="inlineStr">

</xml_diff>